<commit_message>
Doubled up MAG_SDA and MAG_SCL on backplane connector to match backplane, and added pull up resistors for these signals. Updated BOM to reflect this.
</commit_message>
<xml_diff>
--- a/oresat-acs-card-bom.xlsx
+++ b/oresat-acs-card-bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monke\Documents\Oresat_Git\oresat-acs-board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C01EBBE-5E1E-4E93-A612-9AD294B49067}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D8C465-8C36-4AE6-A957-C503AE40A4CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!$A$7:$I$52</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="220">
   <si>
     <t>Description</t>
   </si>
@@ -385,21 +384,6 @@
     <t>U31</t>
   </si>
   <si>
-    <t>Bill Of Materials for OreSat Prototype Card</t>
-  </si>
-  <si>
-    <t>source file: oresat-proto-card.sch</t>
-  </si>
-  <si>
-    <t>Last modified: 2020/01/07</t>
-  </si>
-  <si>
-    <t>PCB version: 4.0</t>
-  </si>
-  <si>
-    <t>BOM revision: 1</t>
-  </si>
-  <si>
     <t>P/DNP</t>
   </si>
   <si>
@@ -475,9 +459,6 @@
     <t>RC0603FR-0710KL</t>
   </si>
   <si>
-    <t>R1, R3, R4, R5, R7, R9, R10, R214, R215, R216, R218, R223, R226, R227, R268, R272</t>
-  </si>
-  <si>
     <t>RES SMD 10K OHM 1% 1/10W 0603</t>
   </si>
   <si>
@@ -686,14 +667,39 @@
   </si>
   <si>
     <t>WM9218CT-ND</t>
+  </si>
+  <si>
+    <t>R1, R3, R4, R5, R6, R7, R9, R10, R13, R214, R215, R216, R218, R223, R226, R227, R268, R272</t>
+  </si>
+  <si>
+    <t>Bill Of Materials for OreSat ACS Card</t>
+  </si>
+  <si>
+    <t>source file: oresat-acs-card.sch</t>
+  </si>
+  <si>
+    <t>Last modified: 2020/09/08</t>
+  </si>
+  <si>
+    <t>PCB version: 1.1</t>
+  </si>
+  <si>
+    <t>BOM revision: 2</t>
+  </si>
+  <si>
+    <t>1.1r0</t>
+  </si>
+  <si>
+    <t>BOM for 1.1r0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="mm/dd/yy"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="167" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -1183,17 +1189,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1242,11 +1249,7 @@
   <dxfs count="11">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1257,24 +1260,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Sans"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1292,7 +1277,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1387,6 +1376,24 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Sans"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1437,18 +1444,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="a" displayName="a" ref="A7:I52" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="a" displayName="a" ref="A7:I52" tableType="queryTable" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A7:I52" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Cnt" queryTableFieldId="1" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Part References" queryTableFieldId="5" dataDxfId="9"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" uniqueName="24" name="P/DNP" queryTableFieldId="25" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" uniqueName="13" name="Mfg" queryTableFieldId="13" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" uniqueName="15" name="Mfg PN" queryTableFieldId="15" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Description" queryTableFieldId="2" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{2E44C4E0-CA1A-40F6-898F-BBBF225C939B}" uniqueName="4" name="Generic" queryTableFieldId="28" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="9" name="DIS" queryTableFieldId="9" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="10" name="DPN" queryTableFieldId="10" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Cnt" queryTableFieldId="1" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Part References" queryTableFieldId="5" dataDxfId="7"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" uniqueName="24" name="P/DNP" queryTableFieldId="25" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" uniqueName="13" name="Mfg" queryTableFieldId="13" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" uniqueName="15" name="Mfg PN" queryTableFieldId="15" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Description" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{2E44C4E0-CA1A-40F6-898F-BBBF225C939B}" uniqueName="4" name="Generic" queryTableFieldId="28" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="9" name="DIS" queryTableFieldId="9" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="10" name="DPN" queryTableFieldId="10" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1751,10 +1758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1775,40 +1782,40 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>118</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>119</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>120</v>
+        <v>216</v>
       </c>
       <c r="D4" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>121</v>
+        <v>217</v>
       </c>
       <c r="D5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E5" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -1817,25 +1824,25 @@
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1">
       <c r="A7" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>1</v>
@@ -1852,7 +1859,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>7</v>
@@ -1861,10 +1868,10 @@
         <v>8</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>5</v>
@@ -1881,25 +1888,25 @@
         <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1910,25 +1917,25 @@
         <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1939,7 +1946,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>7</v>
@@ -1948,10 +1955,10 @@
         <v>12</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>5</v>
@@ -1968,25 +1975,25 @@
         <v>14</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1997,7 +2004,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>17</v>
@@ -2006,10 +2013,10 @@
         <v>18</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>5</v>
@@ -2026,7 +2033,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>21</v>
@@ -2035,10 +2042,10 @@
         <v>22</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>5</v>
@@ -2055,25 +2062,25 @@
         <v>23</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2084,7 +2091,7 @@
         <v>24</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>7</v>
@@ -2093,10 +2100,10 @@
         <v>26</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>5</v>
@@ -2107,31 +2114,31 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="2">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>147</v>
+        <v>212</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -2142,7 +2149,7 @@
         <v>27</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>21</v>
@@ -2151,10 +2158,10 @@
         <v>29</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>5</v>
@@ -2171,7 +2178,7 @@
         <v>31</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>33</v>
@@ -2183,7 +2190,7 @@
         <v>30</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>5</v>
@@ -2200,7 +2207,7 @@
         <v>35</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>7</v>
@@ -2209,10 +2216,10 @@
         <v>37</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>5</v>
@@ -2229,25 +2236,25 @@
         <v>38</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -2255,10 +2262,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>7</v>
@@ -2267,10 +2274,10 @@
         <v>40</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>5</v>
@@ -2284,10 +2291,10 @@
         <v>8</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>42</v>
@@ -2296,10 +2303,10 @@
         <v>43</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>5</v>
@@ -2313,28 +2320,28 @@
         <v>6</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -2345,25 +2352,25 @@
         <v>45</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -2374,7 +2381,7 @@
         <v>46</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>48</v>
@@ -2383,10 +2390,10 @@
         <v>49</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>5</v>
@@ -2403,25 +2410,25 @@
         <v>50</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2432,7 +2439,7 @@
         <v>51</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>53</v>
@@ -2441,10 +2448,10 @@
         <v>54</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>5</v>
@@ -2461,25 +2468,25 @@
         <v>55</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>53</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -2490,7 +2497,7 @@
         <v>56</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>7</v>
@@ -2499,10 +2506,10 @@
         <v>58</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>5</v>
@@ -2519,7 +2526,7 @@
         <v>59</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>61</v>
@@ -2528,10 +2535,10 @@
         <v>62</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>5</v>
@@ -2548,7 +2555,7 @@
         <v>63</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>65</v>
@@ -2557,10 +2564,10 @@
         <v>66</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>5</v>
@@ -2577,7 +2584,7 @@
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>69</v>
@@ -2586,16 +2593,16 @@
         <v>67</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -2606,7 +2613,7 @@
         <v>72</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>74</v>
@@ -2615,10 +2622,10 @@
         <v>70</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>5</v>
@@ -2635,7 +2642,7 @@
         <v>75</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>77</v>
@@ -2644,10 +2651,10 @@
         <v>78</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>5</v>
@@ -2664,7 +2671,7 @@
         <v>80</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>81</v>
@@ -2676,13 +2683,13 @@
         <v>79</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2693,25 +2700,25 @@
         <v>83</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -2722,7 +2729,7 @@
         <v>85</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>87</v>
@@ -2731,10 +2738,10 @@
         <v>84</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>5</v>
@@ -2751,7 +2758,7 @@
         <v>89</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>87</v>
@@ -2760,10 +2767,10 @@
         <v>88</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>5</v>
@@ -2780,25 +2787,25 @@
         <v>91</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>87</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -2809,25 +2816,25 @@
         <v>92</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -2838,25 +2845,25 @@
         <v>93</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -2867,7 +2874,7 @@
         <v>94</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>74</v>
@@ -2879,7 +2886,7 @@
         <v>71</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>5</v>
@@ -2908,7 +2915,7 @@
         <v>97</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>3</v>
@@ -2937,7 +2944,7 @@
         <v>97</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>3</v>
@@ -2962,7 +2969,7 @@
         <v>97</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -2983,7 +2990,7 @@
         <v>97</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -2996,10 +3003,10 @@
         <v>103</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>3</v>
@@ -3008,7 +3015,7 @@
         <v>102</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>3</v>
@@ -3025,7 +3032,7 @@
         <v>104</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>106</v>
@@ -3034,10 +3041,10 @@
         <v>107</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>5</v>
@@ -3054,7 +3061,7 @@
         <v>108</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>110</v>
@@ -3063,10 +3070,10 @@
         <v>111</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>5</v>
@@ -3083,7 +3090,7 @@
         <v>112</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>114</v>
@@ -3092,10 +3099,10 @@
         <v>115</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>5</v>
@@ -3112,54 +3119,65 @@
         <v>116</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>114</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>5</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="B55" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C55" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>173</v>
-      </c>
-      <c r="B57" s="5">
+        <v>218</v>
+      </c>
+      <c r="B57" s="8">
+        <v>44082</v>
+      </c>
+      <c r="C57" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="s">
+        <v>167</v>
+      </c>
+      <c r="B58" s="5">
         <v>44036</v>
       </c>
-      <c r="C57" t="s">
-        <v>174</v>
+      <c r="C58" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed attributes and updated BOM. Also doubled up backplane connector lines and added some test points.
</commit_message>
<xml_diff>
--- a/oresat-acs-card-bom.xlsx
+++ b/oresat-acs-card-bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monke\Documents\Oresat_Git\oresat-acs-board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D8C465-8C36-4AE6-A957-C503AE40A4CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59CB75D-5240-4E8B-8E64-07163DB9FFBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!$A$7:$I$52</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!$A$7:$I$44</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="195">
   <si>
     <t>Description</t>
   </si>
@@ -45,39 +45,12 @@
     <t/>
   </si>
   <si>
-    <t>R59, R61, R97, R99, R173, R175, R249, R251</t>
-  </si>
-  <si>
     <t>Digi-Key</t>
   </si>
   <si>
-    <t>311-0.0JRCT-ND</t>
-  </si>
-  <si>
     <t>Yageo</t>
   </si>
   <si>
-    <t>RC0402JR-070RL</t>
-  </si>
-  <si>
-    <t>R219, R221</t>
-  </si>
-  <si>
-    <t>R200</t>
-  </si>
-  <si>
-    <t>311-100LRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-07100RL</t>
-  </si>
-  <si>
-    <t>R40, R53, R73, R78, R91, R111, R154, R167, R187, R230, R243, R263</t>
-  </si>
-  <si>
-    <t>R213, R271</t>
-  </si>
-  <si>
     <t>R57, R95, R171, R217, R247</t>
   </si>
   <si>
@@ -90,30 +63,9 @@
     <t>CSR1206FTR100</t>
   </si>
   <si>
-    <t>C6, C11, C21, C31</t>
-  </si>
-  <si>
-    <t>1276-1001-1-ND</t>
-  </si>
-  <si>
     <t>Samsung</t>
   </si>
   <si>
-    <t>CL05B104KO5NNNC</t>
-  </si>
-  <si>
-    <t>C28, C29, C37, C38, C39, C43</t>
-  </si>
-  <si>
-    <t>R54, R55, R56, R58, R63, R66, R68, R74, R92, R93, R94, R96, R101, R104, R106, R112, R168, R169, R170, R172, R177, R180, R182, R188, R244, R245, R246, R248, R253, R256, R258, R264</t>
-  </si>
-  <si>
-    <t>311-10.0KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-0710KL</t>
-  </si>
-  <si>
     <t>C45</t>
   </si>
   <si>
@@ -123,9 +75,6 @@
     <t>CL21B106KOQNNNG</t>
   </si>
   <si>
-    <t>16MHZ-2.5x2mm</t>
-  </si>
-  <si>
     <t>X2</t>
   </si>
   <si>
@@ -138,33 +87,12 @@
     <t>ECS-160-10-36Q-ES-TR</t>
   </si>
   <si>
-    <t>R72, R76, R110, R114, R186, R190, R262, R266</t>
-  </si>
-  <si>
-    <t>311-1.00MLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-071ML</t>
-  </si>
-  <si>
-    <t>R270, R274</t>
-  </si>
-  <si>
     <t>311-1446-1-ND</t>
   </si>
   <si>
     <t>CC0603KRX7R7BB105</t>
   </si>
   <si>
-    <t>A129632CT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TE Connectivity </t>
-  </si>
-  <si>
-    <t>CRGCQ0402F2K7</t>
-  </si>
-  <si>
     <t>TE Connectivity</t>
   </si>
   <si>
@@ -186,30 +114,12 @@
     <t>R2</t>
   </si>
   <si>
-    <t>R71, R75, R109, R113, R185, R189, R261, R265</t>
-  </si>
-  <si>
-    <t>749-1575-1-ND</t>
-  </si>
-  <si>
     <t>Vishay</t>
   </si>
   <si>
-    <t>MCS04020C3303FE000</t>
-  </si>
-  <si>
-    <t>R269, R273</t>
-  </si>
-  <si>
     <t>R69, R70, R107, R108, R183, R184, R259, R260</t>
   </si>
   <si>
-    <t>311-47.0KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-0747KL</t>
-  </si>
-  <si>
     <t>L3</t>
   </si>
   <si>
@@ -327,18 +237,6 @@
     <t>NP</t>
   </si>
   <si>
-    <t>C7, C12, C22, C32</t>
-  </si>
-  <si>
-    <t>C44</t>
-  </si>
-  <si>
-    <t>R41, R42, R43, R44, R45, R46, R47, R48, R49, R50, R51, R52, R60, R62, R64, R65, R79, R80, R81, R82, R83, R84, R85, R86, R87, R88, R89, R90, R98, R100, R102, R103, R155, R156, R157, R158, R159, R160, R161, R162, R163, R164, R165, R166, R174, R176, R178, R179, R231, R232, R233, R234, R235, R236, R237, R238, R239, R240, R241, R242, R250, R252, R254, R255</t>
-  </si>
-  <si>
-    <t>R201, R202, R203, R204, R205, R206, R207, R208, R209, R210, R211, R212, R220, R222, R224, R225, R228</t>
-  </si>
-  <si>
     <t>ORESAT-DEBUG-CONNECTOR-SOLAR</t>
   </si>
   <si>
@@ -417,9 +315,6 @@
     <t>Microchip</t>
   </si>
   <si>
-    <t>RES SMD 0 OHM JUMPER 1/16W 0402</t>
-  </si>
-  <si>
     <t>Wurth</t>
   </si>
   <si>
@@ -429,9 +324,6 @@
     <t>RES SMD 0 OHM JUMPER 1/10W 0603</t>
   </si>
   <si>
-    <t>RES SMD 100 OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
     <t>RC0603FR-07100RL</t>
   </si>
   <si>
@@ -462,9 +354,6 @@
     <t>RES SMD 10K OHM 1% 1/10W 0603</t>
   </si>
   <si>
-    <t>RES SMD 10K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
     <t>CAP CER 10UF 16V X7R 0805</t>
   </si>
   <si>
@@ -477,33 +366,18 @@
     <t>311-1.00MHRCT-ND</t>
   </si>
   <si>
-    <t>RES SMD 1M OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
     <t>C1, C2, C3, C4, C8, C9, C10, C13, C14, C15, C16, C23, C24, C25, C33, C34, C35, C46, C48, C49, C50</t>
   </si>
   <si>
     <t>CAP CER 1UF 16V X7R 0603</t>
   </si>
   <si>
-    <t>R39, R67, R77, R105, R153,  R181, R229, R257</t>
-  </si>
-  <si>
     <t>A129693CT-ND</t>
   </si>
   <si>
     <t>CRGCQ0603F2K7</t>
   </si>
   <si>
-    <t>CRGCQ 0603 2K7 1%</t>
-  </si>
-  <si>
-    <t>CRGCQ 0402 2K7 1%</t>
-  </si>
-  <si>
-    <t>R8, R11, R12, R198, R199, R297</t>
-  </si>
-  <si>
     <t>RC0603FR-0723K7L</t>
   </si>
   <si>
@@ -543,9 +417,6 @@
     <t>RES 0.1 OHM 1% 1/2W 1206</t>
   </si>
   <si>
-    <t>CAP CER 0.1UF 16V X7R 0402</t>
-  </si>
-  <si>
     <t>CL10B104KB8NNNL</t>
   </si>
   <si>
@@ -570,21 +441,12 @@
     <t>RES SMD 23.7K OHM 1% 1/10W 0603</t>
   </si>
   <si>
-    <t>RES SMD 330K OHM 1% 1/10W 0402</t>
-  </si>
-  <si>
-    <t>MCT06030C3303FP500</t>
-  </si>
-  <si>
     <t>RES SMD 330K OHM 1% 1/8W 0603</t>
   </si>
   <si>
     <t>749-1638-1-ND</t>
   </si>
   <si>
-    <t>RES SMD 47K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
     <t>828-1082-1-ND</t>
   </si>
   <si>
@@ -651,12 +513,6 @@
     <t>MAX892LEUA+-ND</t>
   </si>
   <si>
-    <t>296-20670-1-ND</t>
-  </si>
-  <si>
-    <t>TPS62111RSAT</t>
-  </si>
-  <si>
     <t>Molex</t>
   </si>
   <si>
@@ -669,18 +525,12 @@
     <t>WM9218CT-ND</t>
   </si>
   <si>
-    <t>R1, R3, R4, R5, R6, R7, R9, R10, R13, R214, R215, R216, R218, R223, R226, R227, R268, R272</t>
-  </si>
-  <si>
     <t>Bill Of Materials for OreSat ACS Card</t>
   </si>
   <si>
     <t>source file: oresat-acs-card.sch</t>
   </si>
   <si>
-    <t>Last modified: 2020/09/08</t>
-  </si>
-  <si>
     <t>PCB version: 1.1</t>
   </si>
   <si>
@@ -691,6 +541,81 @@
   </si>
   <si>
     <t>BOM for 1.1r0</t>
+  </si>
+  <si>
+    <t>R59, R61, R97, R99, R173, R175, R219, R221, R249, R251</t>
+  </si>
+  <si>
+    <t>R40, R78, R154, R200, R230</t>
+  </si>
+  <si>
+    <t>R53, R73, R91, R111, R167, R187, R213, R243, R263, R271</t>
+  </si>
+  <si>
+    <t>C6, C11, C21, C28, C29, C31, C37, C38, C39, C43</t>
+  </si>
+  <si>
+    <t>R1, R3, R4, R5, R6, R7, R9, R10, R13, R54, R55, R56, R58, R63, R66, R92, R93, R94, R96, R101, R104, R168, R169, R170, R172, R177, R180, R214, R215, R216, R218, R223, R226, R227, R244, R245, R246, R248, R253, R256</t>
+  </si>
+  <si>
+    <t>R72, R76, R110, R114, R186, R190, R262, R266, R270, R274</t>
+  </si>
+  <si>
+    <t>R8, R11, R12, R39, R67, R77, R105, R153, R181, R198, R199, R229, R257, R267</t>
+  </si>
+  <si>
+    <t>R71, R75, R109, R113, R185, R189, R261, R265, R269, R273</t>
+  </si>
+  <si>
+    <t>R68, R74, R106, R112, R182, R188, R258, R264, R268, R272</t>
+  </si>
+  <si>
+    <t>C7, C12, C22, C32, C44</t>
+  </si>
+  <si>
+    <t>R41, R42, R43, R44, R45, R46, R47, R48, R49, R50, R51, R52, R60, R62, R64, R65, R79, R80, R81, R82, R83, R84, R85, R86, R87, R88, R89, R90, R98, R100, R102, R103, R155, R156, R157, R158, R159, R160, R161, R162, R163, R164, R165, R166, R174, R176, R178, R179, R201, R202, R203, R204, R205, R206, R207, R208, R209, R210, R211, R212, R220, R222, R224, R225, R228, R231, R232, R233, R234, R235, R236, R237, R238, R239, R240, R241, R242, R250, R252, R254, R255</t>
+  </si>
+  <si>
+    <t>MCT06030C3303FP000</t>
+  </si>
+  <si>
+    <t>RC0603FR-0747KL</t>
+  </si>
+  <si>
+    <t>RC0603FR-07665KL</t>
+  </si>
+  <si>
+    <t>TPS62111RSAR</t>
+  </si>
+  <si>
+    <t>16MHz ±30ppm Crystal 10pF 80 Ohms</t>
+  </si>
+  <si>
+    <t>RES CRGCQ 0603 2K7 1%</t>
+  </si>
+  <si>
+    <t>RES SMD 47K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RES SMD 665K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>311-47.0KHRCT-ND</t>
+  </si>
+  <si>
+    <t>311-665KHRCT-ND</t>
+  </si>
+  <si>
+    <t>296-37681-2-ND</t>
+  </si>
+  <si>
+    <t>1.1r1</t>
+  </si>
+  <si>
+    <t>Changed 0402 components to 0603 and updated some values</t>
+  </si>
+  <si>
+    <t>Last modified: 2020/09/21</t>
   </si>
 </sst>
 </file>
@@ -699,7 +624,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="167" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -1199,8 +1124,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1444,8 +1369,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="a" displayName="a" ref="A7:I52" tableType="queryTable" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A7:I52" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="a" displayName="a" ref="A7:I44" tableType="queryTable" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A7:I44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Cnt" queryTableFieldId="1" dataDxfId="8"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Part References" queryTableFieldId="5" dataDxfId="7"/>
@@ -1758,10 +1683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1782,40 +1707,40 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>213</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>214</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>216</v>
+        <v>166</v>
       </c>
       <c r="D4" t="s">
-        <v>159</v>
+        <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>160</v>
+        <v>118</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>217</v>
+        <v>167</v>
       </c>
       <c r="D5" t="s">
-        <v>161</v>
+        <v>119</v>
       </c>
       <c r="E5" t="s">
-        <v>162</v>
+        <v>120</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -1824,25 +1749,25 @@
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1">
       <c r="A7" s="4" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>1</v>
@@ -1853,1331 +1778,1116 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>128</v>
+        <v>84</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>6</v>
+        <v>91</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2">
-        <v>2</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>131</v>
+        <v>84</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>136</v>
+        <v>91</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="2">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>172</v>
+      </c>
       <c r="C10" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>137</v>
+        <v>84</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>139</v>
+        <v>91</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2">
-        <v>12</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D11" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2">
-        <v>2</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>134</v>
+        <v>84</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>135</v>
+        <v>91</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="2">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>169</v>
+      <c r="E13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>16</v>
+        <v>91</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2">
-        <v>4</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>170</v>
+        <v>84</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>20</v>
+        <v>91</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2">
-        <v>6</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>23</v>
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>172</v>
+        <v>84</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>185</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>173</v>
+        <v>91</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="2">
-        <v>32</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>143</v>
+        <v>84</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>25</v>
+        <v>91</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="2">
+        <v>21</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="2">
-        <v>1</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>27</v>
+        <v>14</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>144</v>
+        <v>84</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>28</v>
+        <v>91</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="2">
-        <v>1</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>31</v>
+        <v>2</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>30</v>
+        <v>84</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>32</v>
+        <v>91</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2">
-        <v>8</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>35</v>
+        <v>1</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>148</v>
+        <v>84</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>36</v>
+        <v>91</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="2">
-        <v>2</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>38</v>
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>146</v>
+        <v>84</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>147</v>
+        <v>91</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="2">
-        <v>21</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>149</v>
+        <v>10</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>150</v>
+        <v>84</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>39</v>
+        <v>91</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="2">
         <v>8</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>151</v>
+      <c r="B23" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>155</v>
+        <v>84</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>41</v>
+        <v>91</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="2">
-        <v>6</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>156</v>
+        <v>1</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>154</v>
+        <v>84</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>152</v>
+        <v>92</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="2">
-        <v>2</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>45</v>
+        <v>10</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>176</v>
+        <v>84</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>175</v>
+        <v>91</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="2">
-        <v>1</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>46</v>
+        <v>6</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>177</v>
+        <v>84</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>47</v>
+        <v>91</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="2">
         <v>1</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>50</v>
+      <c r="B27" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>178</v>
+        <v>84</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>158</v>
+        <v>92</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="2">
-        <v>8</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>51</v>
+        <v>5</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>179</v>
+        <v>84</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>52</v>
+        <v>92</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="2">
-        <v>2</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>55</v>
+        <v>6</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>181</v>
+        <v>84</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>182</v>
+        <v>91</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="2">
-        <v>8</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>56</v>
+        <v>1</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>183</v>
+        <v>84</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>57</v>
+        <v>92</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="2">
         <v>1</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>59</v>
+      <c r="B31" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>191</v>
+        <v>84</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>60</v>
+        <v>92</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="2">
-        <v>6</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>63</v>
+        <v>5</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>192</v>
+        <v>84</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>64</v>
+        <v>92</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="2">
-        <v>1</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>68</v>
+        <v>5</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>123</v>
+        <v>84</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>184</v>
+        <v>92</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="2">
-        <v>5</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>72</v>
+        <v>1</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>194</v>
+        <v>84</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>73</v>
+        <v>92</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="2">
-        <v>6</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>75</v>
+        <v>4</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>193</v>
+        <v>84</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>76</v>
+        <v>92</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="2">
-        <v>1</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>80</v>
+        <v>10</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>79</v>
+        <v>84</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>185</v>
+        <v>92</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="2">
-        <v>1</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>83</v>
+        <v>10</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>195</v>
+        <v>84</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>188</v>
+        <v>92</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="2">
         <v>5</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>85</v>
+      <c r="B38" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>196</v>
+        <v>67</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
+      </c>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="2">
-        <v>5</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>197</v>
+        <v>67</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>90</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="2">
         <v>1</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>91</v>
+      <c r="B40" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>204</v>
+        <v>84</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>205</v>
+        <v>92</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="2">
-        <v>4</v>
-      </c>
-      <c r="B41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>211</v>
+      <c r="H41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="2">
-        <v>10</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>93</v>
+        <v>1</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>198</v>
+        <v>84</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>189</v>
+        <v>92</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="2">
-        <v>10</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>94</v>
+        <v>1</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>71</v>
+        <v>84</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="2">
-        <v>4</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>98</v>
+        <v>1</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="G44" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="B47" t="s">
+        <v>122</v>
+      </c>
+      <c r="C47" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>192</v>
+      </c>
+      <c r="B49" s="8">
+        <v>44095</v>
+      </c>
+      <c r="C49" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>168</v>
+      </c>
+      <c r="B50" s="7">
+        <v>44082</v>
+      </c>
+      <c r="C50" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
         <v>125</v>
       </c>
-      <c r="H44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="2">
-        <v>1</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="2">
-        <v>64</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="2">
-        <v>17</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="2">
-        <v>1</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="G48" s="3" t="s">
+      <c r="B51" s="5">
+        <v>44036</v>
+      </c>
+      <c r="C51" t="s">
         <v>126</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="2">
-        <v>10</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="2">
-        <v>1</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="2">
-        <v>1</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="2">
-        <v>1</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="A54" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="B55" t="s">
-        <v>164</v>
-      </c>
-      <c r="C55" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57" t="s">
-        <v>218</v>
-      </c>
-      <c r="B57" s="8">
-        <v>44082</v>
-      </c>
-      <c r="C57" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58" t="s">
-        <v>167</v>
-      </c>
-      <c r="B58" s="5">
-        <v>44036</v>
-      </c>
-      <c r="C58" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>